<commit_message>
continued building out REST examples
</commit_message>
<xml_diff>
--- a/src/test/resources/googleApi/dataProviders/Geocode.xlsx
+++ b/src/test/resources/googleApi/dataProviders/Geocode.xlsx
@@ -4,24 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="195" windowWidth="18195" windowHeight="6915"/>
+    <workbookView xWindow="0" yWindow="195" windowWidth="18195" windowHeight="6915" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Geocode" sheetId="1" r:id="rId1"/>
+    <sheet name="Geocode2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="23">
   <si>
     <t>TestScenario</t>
   </si>
   <si>
-    <t>Test1234</t>
-  </si>
-  <si>
     <t>Domestic Address</t>
   </si>
   <si>
@@ -68,6 +66,24 @@
   </si>
   <si>
     <t>StreetNumberTarget</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>xml</t>
+  </si>
+  <si>
+    <t>Albert Pick Road</t>
+  </si>
+  <si>
+    <t>7025</t>
+  </si>
+  <si>
+    <t>27409</t>
+  </si>
+  <si>
+    <t>json</t>
   </si>
 </sst>
 </file>
@@ -552,8 +568,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -896,10 +913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection sqref="A1:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,7 +924,7 @@
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -915,68 +932,207 @@
     <col min="10" max="10" width="38.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>7025</v>
       </c>
       <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
       </c>
       <c r="F2">
         <v>27409</v>
       </c>
       <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
         <v>11</v>
       </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
       <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
         <v>14</v>
       </c>
-      <c r="J2" t="s">
-        <v>16</v>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
began building out SOAP examples
</commit_message>
<xml_diff>
--- a/src/test/resources/googleApi/dataProviders/Geocode.xlsx
+++ b/src/test/resources/googleApi/dataProviders/Geocode.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="195" windowWidth="18195" windowHeight="6915" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="195" windowWidth="18195" windowHeight="6915"/>
   </bookViews>
   <sheets>
     <sheet name="Geocode" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="23">
   <si>
     <t>TestScenario</t>
   </si>
@@ -913,10 +913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection sqref="A1:K2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,8 +971,8 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>7025</v>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -983,8 +983,8 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="F2">
-        <v>27409</v>
+      <c r="F2" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
@@ -1000,6 +1000,41 @@
       </c>
       <c r="K2" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1011,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>